<commit_message>
issues 9 and 10, fixed.
</commit_message>
<xml_diff>
--- a/surf-forecaster/gui/resources/Partitions.xlsx
+++ b/surf-forecaster/gui/resources/Partitions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1986" uniqueCount="283">
   <si>
     <t>P1</t>
   </si>
@@ -856,6 +856,15 @@
   </si>
   <si>
     <t>P264</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>"+</t>
+  </si>
+  <si>
+    <t>')),</t>
   </si>
 </sst>
 </file>
@@ -863,7 +872,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -896,7 +905,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,10 +1201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F368"/>
+  <dimension ref="A1:P368"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A264" sqref="A264"/>
+    <sheetView tabSelected="1" topLeftCell="D265" workbookViewId="0">
+      <selection activeCell="I154" sqref="I154:P264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1206,6 +1215,8 @@
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -4088,7 +4099,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="145" spans="1:6">
+    <row r="145" spans="1:16">
       <c r="A145" t="s">
         <v>16</v>
       </c>
@@ -4108,7 +4119,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:16">
       <c r="A146" t="s">
         <v>16</v>
       </c>
@@ -4128,7 +4139,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:16">
       <c r="A147" t="s">
         <v>16</v>
       </c>
@@ -4148,7 +4159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:16">
       <c r="A148" t="s">
         <v>16</v>
       </c>
@@ -4168,7 +4179,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:16">
       <c r="A149" t="s">
         <v>16</v>
       </c>
@@ -4188,7 +4199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:6">
+    <row r="150" spans="1:16">
       <c r="A150" t="s">
         <v>16</v>
       </c>
@@ -4208,7 +4219,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:6">
+    <row r="151" spans="1:16">
       <c r="A151" t="s">
         <v>16</v>
       </c>
@@ -4228,7 +4239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="1:6">
+    <row r="152" spans="1:16">
       <c r="A152" t="s">
         <v>16</v>
       </c>
@@ -4248,7 +4259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:16">
       <c r="A153" t="s">
         <v>16</v>
       </c>
@@ -4268,7 +4279,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="154" spans="1:6">
+    <row r="154" spans="1:16">
       <c r="A154" t="s">
         <v>16</v>
       </c>
@@ -4287,8 +4298,29 @@
       <c r="F154" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="155" spans="1:6">
+      <c r="I154" t="s">
+        <v>280</v>
+      </c>
+      <c r="J154" t="s">
+        <v>16</v>
+      </c>
+      <c r="K154" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L154" t="s">
+        <v>17</v>
+      </c>
+      <c r="M154" s="1">
+        <v>40118</v>
+      </c>
+      <c r="N154" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P154" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16">
       <c r="A155" t="s">
         <v>16</v>
       </c>
@@ -4307,8 +4339,29 @@
       <c r="F155" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="156" spans="1:6">
+      <c r="I155" t="s">
+        <v>280</v>
+      </c>
+      <c r="J155" t="s">
+        <v>16</v>
+      </c>
+      <c r="K155" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L155" t="s">
+        <v>17</v>
+      </c>
+      <c r="M155" s="1">
+        <v>40148</v>
+      </c>
+      <c r="N155" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P155" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16">
       <c r="A156" t="s">
         <v>16</v>
       </c>
@@ -4327,8 +4380,29 @@
       <c r="F156" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="157" spans="1:6">
+      <c r="I156" t="s">
+        <v>280</v>
+      </c>
+      <c r="J156" t="s">
+        <v>16</v>
+      </c>
+      <c r="K156" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L156" t="s">
+        <v>17</v>
+      </c>
+      <c r="M156" s="1">
+        <v>40179</v>
+      </c>
+      <c r="N156" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P156" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="157" spans="1:16">
       <c r="A157" t="s">
         <v>16</v>
       </c>
@@ -4347,8 +4421,29 @@
       <c r="F157" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="158" spans="1:6">
+      <c r="I157" t="s">
+        <v>280</v>
+      </c>
+      <c r="J157" t="s">
+        <v>16</v>
+      </c>
+      <c r="K157" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L157" t="s">
+        <v>17</v>
+      </c>
+      <c r="M157" s="1">
+        <v>40210</v>
+      </c>
+      <c r="N157" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P157" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="158" spans="1:16">
       <c r="A158" t="s">
         <v>16</v>
       </c>
@@ -4367,8 +4462,29 @@
       <c r="F158" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="159" spans="1:6">
+      <c r="I158" t="s">
+        <v>280</v>
+      </c>
+      <c r="J158" t="s">
+        <v>16</v>
+      </c>
+      <c r="K158" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L158" t="s">
+        <v>17</v>
+      </c>
+      <c r="M158" s="1">
+        <v>40238</v>
+      </c>
+      <c r="N158" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P158" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="159" spans="1:16">
       <c r="A159" t="s">
         <v>16</v>
       </c>
@@ -4387,8 +4503,29 @@
       <c r="F159" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="160" spans="1:6">
+      <c r="I159" t="s">
+        <v>280</v>
+      </c>
+      <c r="J159" t="s">
+        <v>16</v>
+      </c>
+      <c r="K159" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L159" t="s">
+        <v>17</v>
+      </c>
+      <c r="M159" s="1">
+        <v>40269</v>
+      </c>
+      <c r="N159" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P159" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="160" spans="1:16">
       <c r="A160" t="s">
         <v>16</v>
       </c>
@@ -4407,8 +4544,29 @@
       <c r="F160" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="161" spans="1:6">
+      <c r="I160" t="s">
+        <v>280</v>
+      </c>
+      <c r="J160" t="s">
+        <v>16</v>
+      </c>
+      <c r="K160" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L160" t="s">
+        <v>17</v>
+      </c>
+      <c r="M160" s="1">
+        <v>40299</v>
+      </c>
+      <c r="N160" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P160" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="161" spans="1:16">
       <c r="A161" t="s">
         <v>16</v>
       </c>
@@ -4427,8 +4585,29 @@
       <c r="F161" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="162" spans="1:6">
+      <c r="I161" t="s">
+        <v>280</v>
+      </c>
+      <c r="J161" t="s">
+        <v>16</v>
+      </c>
+      <c r="K161" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L161" t="s">
+        <v>17</v>
+      </c>
+      <c r="M161" s="1">
+        <v>40330</v>
+      </c>
+      <c r="N161" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P161" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="162" spans="1:16">
       <c r="A162" t="s">
         <v>16</v>
       </c>
@@ -4447,8 +4626,29 @@
       <c r="F162" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="163" spans="1:6">
+      <c r="I162" t="s">
+        <v>280</v>
+      </c>
+      <c r="J162" t="s">
+        <v>16</v>
+      </c>
+      <c r="K162" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L162" t="s">
+        <v>17</v>
+      </c>
+      <c r="M162" s="1">
+        <v>40360</v>
+      </c>
+      <c r="N162" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P162" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="163" spans="1:16">
       <c r="A163" t="s">
         <v>16</v>
       </c>
@@ -4467,8 +4667,29 @@
       <c r="F163" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="164" spans="1:6">
+      <c r="I163" t="s">
+        <v>280</v>
+      </c>
+      <c r="J163" t="s">
+        <v>16</v>
+      </c>
+      <c r="K163" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L163" t="s">
+        <v>17</v>
+      </c>
+      <c r="M163" s="1">
+        <v>40391</v>
+      </c>
+      <c r="N163" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P163" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="164" spans="1:16">
       <c r="A164" t="s">
         <v>16</v>
       </c>
@@ -4487,8 +4708,29 @@
       <c r="F164" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="165" spans="1:6">
+      <c r="I164" t="s">
+        <v>280</v>
+      </c>
+      <c r="J164" t="s">
+        <v>16</v>
+      </c>
+      <c r="K164" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L164" t="s">
+        <v>17</v>
+      </c>
+      <c r="M164" s="1">
+        <v>40422</v>
+      </c>
+      <c r="N164" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P164" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="165" spans="1:16">
       <c r="A165" t="s">
         <v>16</v>
       </c>
@@ -4507,8 +4749,29 @@
       <c r="F165" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="166" spans="1:6">
+      <c r="I165" t="s">
+        <v>280</v>
+      </c>
+      <c r="J165" t="s">
+        <v>16</v>
+      </c>
+      <c r="K165" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L165" t="s">
+        <v>17</v>
+      </c>
+      <c r="M165" s="1">
+        <v>40452</v>
+      </c>
+      <c r="N165" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P165" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="166" spans="1:16">
       <c r="A166" t="s">
         <v>16</v>
       </c>
@@ -4527,8 +4790,29 @@
       <c r="F166" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="167" spans="1:6">
+      <c r="I166" t="s">
+        <v>280</v>
+      </c>
+      <c r="J166" t="s">
+        <v>16</v>
+      </c>
+      <c r="K166" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L166" t="s">
+        <v>17</v>
+      </c>
+      <c r="M166" s="1">
+        <v>40483</v>
+      </c>
+      <c r="N166" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P166" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="167" spans="1:16">
       <c r="A167" t="s">
         <v>16</v>
       </c>
@@ -4547,8 +4831,29 @@
       <c r="F167" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="168" spans="1:6">
+      <c r="I167" t="s">
+        <v>280</v>
+      </c>
+      <c r="J167" t="s">
+        <v>16</v>
+      </c>
+      <c r="K167" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L167" t="s">
+        <v>17</v>
+      </c>
+      <c r="M167" s="1">
+        <v>40513</v>
+      </c>
+      <c r="N167" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P167" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="168" spans="1:16">
       <c r="A168" t="s">
         <v>16</v>
       </c>
@@ -4567,8 +4872,29 @@
       <c r="F168" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="169" spans="1:6">
+      <c r="I168" t="s">
+        <v>280</v>
+      </c>
+      <c r="J168" t="s">
+        <v>16</v>
+      </c>
+      <c r="K168" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L168" t="s">
+        <v>17</v>
+      </c>
+      <c r="M168" s="1">
+        <v>40544</v>
+      </c>
+      <c r="N168" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P168" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="169" spans="1:16">
       <c r="A169" t="s">
         <v>16</v>
       </c>
@@ -4587,8 +4913,29 @@
       <c r="F169" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="170" spans="1:6">
+      <c r="I169" t="s">
+        <v>280</v>
+      </c>
+      <c r="J169" t="s">
+        <v>16</v>
+      </c>
+      <c r="K169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L169" t="s">
+        <v>17</v>
+      </c>
+      <c r="M169" s="1">
+        <v>40575</v>
+      </c>
+      <c r="N169" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P169" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="170" spans="1:16">
       <c r="A170" t="s">
         <v>16</v>
       </c>
@@ -4607,8 +4954,29 @@
       <c r="F170" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="171" spans="1:6">
+      <c r="I170" t="s">
+        <v>280</v>
+      </c>
+      <c r="J170" t="s">
+        <v>16</v>
+      </c>
+      <c r="K170" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L170" t="s">
+        <v>17</v>
+      </c>
+      <c r="M170" s="1">
+        <v>40603</v>
+      </c>
+      <c r="N170" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P170" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="171" spans="1:16">
       <c r="A171" t="s">
         <v>16</v>
       </c>
@@ -4627,8 +4995,29 @@
       <c r="F171" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="172" spans="1:6">
+      <c r="I171" t="s">
+        <v>280</v>
+      </c>
+      <c r="J171" t="s">
+        <v>16</v>
+      </c>
+      <c r="K171" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L171" t="s">
+        <v>17</v>
+      </c>
+      <c r="M171" s="1">
+        <v>40634</v>
+      </c>
+      <c r="N171" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P171" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="172" spans="1:16">
       <c r="A172" t="s">
         <v>16</v>
       </c>
@@ -4647,8 +5036,29 @@
       <c r="F172" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="173" spans="1:6">
+      <c r="I172" t="s">
+        <v>280</v>
+      </c>
+      <c r="J172" t="s">
+        <v>16</v>
+      </c>
+      <c r="K172" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L172" t="s">
+        <v>17</v>
+      </c>
+      <c r="M172" s="1">
+        <v>40664</v>
+      </c>
+      <c r="N172" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P172" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="173" spans="1:16">
       <c r="A173" t="s">
         <v>16</v>
       </c>
@@ -4667,8 +5077,29 @@
       <c r="F173" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="174" spans="1:6">
+      <c r="I173" t="s">
+        <v>280</v>
+      </c>
+      <c r="J173" t="s">
+        <v>16</v>
+      </c>
+      <c r="K173" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L173" t="s">
+        <v>17</v>
+      </c>
+      <c r="M173" s="1">
+        <v>40695</v>
+      </c>
+      <c r="N173" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P173" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="174" spans="1:16">
       <c r="A174" t="s">
         <v>16</v>
       </c>
@@ -4687,8 +5118,29 @@
       <c r="F174" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="175" spans="1:6">
+      <c r="I174" t="s">
+        <v>280</v>
+      </c>
+      <c r="J174" t="s">
+        <v>16</v>
+      </c>
+      <c r="K174" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L174" t="s">
+        <v>17</v>
+      </c>
+      <c r="M174" s="1">
+        <v>40725</v>
+      </c>
+      <c r="N174" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P174" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="175" spans="1:16">
       <c r="A175" t="s">
         <v>16</v>
       </c>
@@ -4707,8 +5159,29 @@
       <c r="F175" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="176" spans="1:6">
+      <c r="I175" t="s">
+        <v>280</v>
+      </c>
+      <c r="J175" t="s">
+        <v>16</v>
+      </c>
+      <c r="K175" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L175" t="s">
+        <v>17</v>
+      </c>
+      <c r="M175" s="1">
+        <v>40756</v>
+      </c>
+      <c r="N175" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P175" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="176" spans="1:16">
       <c r="A176" t="s">
         <v>16</v>
       </c>
@@ -4727,8 +5200,29 @@
       <c r="F176" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="177" spans="1:6">
+      <c r="I176" t="s">
+        <v>280</v>
+      </c>
+      <c r="J176" t="s">
+        <v>16</v>
+      </c>
+      <c r="K176" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L176" t="s">
+        <v>17</v>
+      </c>
+      <c r="M176" s="1">
+        <v>40787</v>
+      </c>
+      <c r="N176" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P176" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="177" spans="1:16">
       <c r="A177" t="s">
         <v>16</v>
       </c>
@@ -4747,8 +5241,29 @@
       <c r="F177" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="178" spans="1:6">
+      <c r="I177" t="s">
+        <v>280</v>
+      </c>
+      <c r="J177" t="s">
+        <v>16</v>
+      </c>
+      <c r="K177" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L177" t="s">
+        <v>17</v>
+      </c>
+      <c r="M177" s="1">
+        <v>40817</v>
+      </c>
+      <c r="N177" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P177" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="178" spans="1:16">
       <c r="A178" t="s">
         <v>16</v>
       </c>
@@ -4767,8 +5282,29 @@
       <c r="F178" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="179" spans="1:6">
+      <c r="I178" t="s">
+        <v>280</v>
+      </c>
+      <c r="J178" t="s">
+        <v>16</v>
+      </c>
+      <c r="K178" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L178" t="s">
+        <v>17</v>
+      </c>
+      <c r="M178" s="1">
+        <v>40848</v>
+      </c>
+      <c r="N178" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P178" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="179" spans="1:16">
       <c r="A179" t="s">
         <v>16</v>
       </c>
@@ -4787,8 +5323,29 @@
       <c r="F179" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="180" spans="1:6">
+      <c r="I179" t="s">
+        <v>280</v>
+      </c>
+      <c r="J179" t="s">
+        <v>16</v>
+      </c>
+      <c r="K179" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L179" t="s">
+        <v>17</v>
+      </c>
+      <c r="M179" s="1">
+        <v>40878</v>
+      </c>
+      <c r="N179" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P179" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="180" spans="1:16">
       <c r="A180" t="s">
         <v>16</v>
       </c>
@@ -4807,8 +5364,29 @@
       <c r="F180" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="181" spans="1:6">
+      <c r="I180" t="s">
+        <v>280</v>
+      </c>
+      <c r="J180" t="s">
+        <v>16</v>
+      </c>
+      <c r="K180" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L180" t="s">
+        <v>17</v>
+      </c>
+      <c r="M180" s="1">
+        <v>40909</v>
+      </c>
+      <c r="N180" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P180" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="181" spans="1:16">
       <c r="A181" t="s">
         <v>16</v>
       </c>
@@ -4827,8 +5405,29 @@
       <c r="F181" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="182" spans="1:6">
+      <c r="I181" t="s">
+        <v>280</v>
+      </c>
+      <c r="J181" t="s">
+        <v>16</v>
+      </c>
+      <c r="K181" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L181" t="s">
+        <v>17</v>
+      </c>
+      <c r="M181" s="1">
+        <v>40940</v>
+      </c>
+      <c r="N181" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P181" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="182" spans="1:16">
       <c r="A182" t="s">
         <v>16</v>
       </c>
@@ -4847,8 +5446,29 @@
       <c r="F182" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="183" spans="1:6">
+      <c r="I182" t="s">
+        <v>280</v>
+      </c>
+      <c r="J182" t="s">
+        <v>16</v>
+      </c>
+      <c r="K182" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L182" t="s">
+        <v>17</v>
+      </c>
+      <c r="M182" s="1">
+        <v>40969</v>
+      </c>
+      <c r="N182" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P182" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="183" spans="1:16">
       <c r="A183" t="s">
         <v>16</v>
       </c>
@@ -4867,8 +5487,29 @@
       <c r="F183" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="184" spans="1:6">
+      <c r="I183" t="s">
+        <v>280</v>
+      </c>
+      <c r="J183" t="s">
+        <v>16</v>
+      </c>
+      <c r="K183" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L183" t="s">
+        <v>17</v>
+      </c>
+      <c r="M183" s="1">
+        <v>41000</v>
+      </c>
+      <c r="N183" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P183" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="184" spans="1:16">
       <c r="A184" t="s">
         <v>16</v>
       </c>
@@ -4887,8 +5528,29 @@
       <c r="F184" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="185" spans="1:6">
+      <c r="I184" t="s">
+        <v>280</v>
+      </c>
+      <c r="J184" t="s">
+        <v>16</v>
+      </c>
+      <c r="K184" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L184" t="s">
+        <v>17</v>
+      </c>
+      <c r="M184" s="1">
+        <v>41030</v>
+      </c>
+      <c r="N184" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P184" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="185" spans="1:16">
       <c r="A185" t="s">
         <v>16</v>
       </c>
@@ -4907,8 +5569,29 @@
       <c r="F185" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="186" spans="1:6">
+      <c r="I185" t="s">
+        <v>280</v>
+      </c>
+      <c r="J185" t="s">
+        <v>16</v>
+      </c>
+      <c r="K185" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L185" t="s">
+        <v>17</v>
+      </c>
+      <c r="M185" s="1">
+        <v>41061</v>
+      </c>
+      <c r="N185" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P185" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="186" spans="1:16">
       <c r="A186" t="s">
         <v>16</v>
       </c>
@@ -4927,8 +5610,29 @@
       <c r="F186" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="187" spans="1:6">
+      <c r="I186" t="s">
+        <v>280</v>
+      </c>
+      <c r="J186" t="s">
+        <v>16</v>
+      </c>
+      <c r="K186" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L186" t="s">
+        <v>17</v>
+      </c>
+      <c r="M186" s="1">
+        <v>41091</v>
+      </c>
+      <c r="N186" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P186" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="187" spans="1:16">
       <c r="A187" t="s">
         <v>16</v>
       </c>
@@ -4947,8 +5651,29 @@
       <c r="F187" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="188" spans="1:6">
+      <c r="I187" t="s">
+        <v>280</v>
+      </c>
+      <c r="J187" t="s">
+        <v>16</v>
+      </c>
+      <c r="K187" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L187" t="s">
+        <v>17</v>
+      </c>
+      <c r="M187" s="1">
+        <v>41122</v>
+      </c>
+      <c r="N187" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P187" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="188" spans="1:16">
       <c r="A188" t="s">
         <v>16</v>
       </c>
@@ -4967,8 +5692,29 @@
       <c r="F188" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="189" spans="1:6">
+      <c r="I188" t="s">
+        <v>280</v>
+      </c>
+      <c r="J188" t="s">
+        <v>16</v>
+      </c>
+      <c r="K188" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L188" t="s">
+        <v>17</v>
+      </c>
+      <c r="M188" s="1">
+        <v>41153</v>
+      </c>
+      <c r="N188" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P188" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="189" spans="1:16">
       <c r="A189" t="s">
         <v>16</v>
       </c>
@@ -4987,8 +5733,29 @@
       <c r="F189" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="190" spans="1:6">
+      <c r="I189" t="s">
+        <v>280</v>
+      </c>
+      <c r="J189" t="s">
+        <v>16</v>
+      </c>
+      <c r="K189" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L189" t="s">
+        <v>17</v>
+      </c>
+      <c r="M189" s="1">
+        <v>41183</v>
+      </c>
+      <c r="N189" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P189" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="190" spans="1:16">
       <c r="A190" t="s">
         <v>16</v>
       </c>
@@ -5007,8 +5774,29 @@
       <c r="F190" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="191" spans="1:6">
+      <c r="I190" t="s">
+        <v>280</v>
+      </c>
+      <c r="J190" t="s">
+        <v>16</v>
+      </c>
+      <c r="K190" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L190" t="s">
+        <v>17</v>
+      </c>
+      <c r="M190" s="1">
+        <v>41214</v>
+      </c>
+      <c r="N190" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P190" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="191" spans="1:16">
       <c r="A191" t="s">
         <v>16</v>
       </c>
@@ -5027,8 +5815,29 @@
       <c r="F191" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="192" spans="1:6">
+      <c r="I191" t="s">
+        <v>280</v>
+      </c>
+      <c r="J191" t="s">
+        <v>16</v>
+      </c>
+      <c r="K191" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L191" t="s">
+        <v>17</v>
+      </c>
+      <c r="M191" s="1">
+        <v>41244</v>
+      </c>
+      <c r="N191" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P191" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="192" spans="1:16">
       <c r="A192" t="s">
         <v>16</v>
       </c>
@@ -5047,8 +5856,29 @@
       <c r="F192" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="193" spans="1:6">
+      <c r="I192" t="s">
+        <v>280</v>
+      </c>
+      <c r="J192" t="s">
+        <v>16</v>
+      </c>
+      <c r="K192" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L192" t="s">
+        <v>17</v>
+      </c>
+      <c r="M192" s="1">
+        <v>41275</v>
+      </c>
+      <c r="N192" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P192" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="193" spans="1:16">
       <c r="A193" t="s">
         <v>16</v>
       </c>
@@ -5067,8 +5897,29 @@
       <c r="F193" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="194" spans="1:6">
+      <c r="I193" t="s">
+        <v>280</v>
+      </c>
+      <c r="J193" t="s">
+        <v>16</v>
+      </c>
+      <c r="K193" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L193" t="s">
+        <v>17</v>
+      </c>
+      <c r="M193" s="1">
+        <v>41306</v>
+      </c>
+      <c r="N193" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P193" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="194" spans="1:16">
       <c r="A194" t="s">
         <v>16</v>
       </c>
@@ -5087,8 +5938,29 @@
       <c r="F194" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="195" spans="1:6">
+      <c r="I194" t="s">
+        <v>280</v>
+      </c>
+      <c r="J194" t="s">
+        <v>16</v>
+      </c>
+      <c r="K194" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L194" t="s">
+        <v>17</v>
+      </c>
+      <c r="M194" s="1">
+        <v>41334</v>
+      </c>
+      <c r="N194" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P194" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="195" spans="1:16">
       <c r="A195" t="s">
         <v>16</v>
       </c>
@@ -5107,8 +5979,29 @@
       <c r="F195" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="196" spans="1:6">
+      <c r="I195" t="s">
+        <v>280</v>
+      </c>
+      <c r="J195" t="s">
+        <v>16</v>
+      </c>
+      <c r="K195" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L195" t="s">
+        <v>17</v>
+      </c>
+      <c r="M195" s="1">
+        <v>41365</v>
+      </c>
+      <c r="N195" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P195" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="196" spans="1:16">
       <c r="A196" t="s">
         <v>16</v>
       </c>
@@ -5127,8 +6020,29 @@
       <c r="F196" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="197" spans="1:6">
+      <c r="I196" t="s">
+        <v>280</v>
+      </c>
+      <c r="J196" t="s">
+        <v>16</v>
+      </c>
+      <c r="K196" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L196" t="s">
+        <v>17</v>
+      </c>
+      <c r="M196" s="1">
+        <v>41395</v>
+      </c>
+      <c r="N196" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P196" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="197" spans="1:16">
       <c r="A197" t="s">
         <v>16</v>
       </c>
@@ -5147,8 +6061,29 @@
       <c r="F197" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="198" spans="1:6">
+      <c r="I197" t="s">
+        <v>280</v>
+      </c>
+      <c r="J197" t="s">
+        <v>16</v>
+      </c>
+      <c r="K197" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L197" t="s">
+        <v>17</v>
+      </c>
+      <c r="M197" s="1">
+        <v>41426</v>
+      </c>
+      <c r="N197" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P197" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="198" spans="1:16">
       <c r="A198" t="s">
         <v>16</v>
       </c>
@@ -5167,8 +6102,29 @@
       <c r="F198" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="199" spans="1:6">
+      <c r="I198" t="s">
+        <v>280</v>
+      </c>
+      <c r="J198" t="s">
+        <v>16</v>
+      </c>
+      <c r="K198" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L198" t="s">
+        <v>17</v>
+      </c>
+      <c r="M198" s="1">
+        <v>41456</v>
+      </c>
+      <c r="N198" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P198" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="199" spans="1:16">
       <c r="A199" t="s">
         <v>16</v>
       </c>
@@ -5187,8 +6143,29 @@
       <c r="F199" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="200" spans="1:6">
+      <c r="I199" t="s">
+        <v>280</v>
+      </c>
+      <c r="J199" t="s">
+        <v>16</v>
+      </c>
+      <c r="K199" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L199" t="s">
+        <v>17</v>
+      </c>
+      <c r="M199" s="1">
+        <v>41487</v>
+      </c>
+      <c r="N199" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P199" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="200" spans="1:16">
       <c r="A200" t="s">
         <v>16</v>
       </c>
@@ -5207,8 +6184,29 @@
       <c r="F200" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="201" spans="1:6">
+      <c r="I200" t="s">
+        <v>280</v>
+      </c>
+      <c r="J200" t="s">
+        <v>16</v>
+      </c>
+      <c r="K200" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L200" t="s">
+        <v>17</v>
+      </c>
+      <c r="M200" s="1">
+        <v>41518</v>
+      </c>
+      <c r="N200" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P200" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="201" spans="1:16">
       <c r="A201" t="s">
         <v>16</v>
       </c>
@@ -5227,8 +6225,29 @@
       <c r="F201" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="202" spans="1:6">
+      <c r="I201" t="s">
+        <v>280</v>
+      </c>
+      <c r="J201" t="s">
+        <v>16</v>
+      </c>
+      <c r="K201" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L201" t="s">
+        <v>17</v>
+      </c>
+      <c r="M201" s="1">
+        <v>41548</v>
+      </c>
+      <c r="N201" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P201" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="202" spans="1:16">
       <c r="A202" t="s">
         <v>16</v>
       </c>
@@ -5247,8 +6266,29 @@
       <c r="F202" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="203" spans="1:6">
+      <c r="I202" t="s">
+        <v>280</v>
+      </c>
+      <c r="J202" t="s">
+        <v>16</v>
+      </c>
+      <c r="K202" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L202" t="s">
+        <v>17</v>
+      </c>
+      <c r="M202" s="1">
+        <v>41579</v>
+      </c>
+      <c r="N202" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P202" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="203" spans="1:16">
       <c r="A203" t="s">
         <v>16</v>
       </c>
@@ -5267,8 +6307,29 @@
       <c r="F203" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="204" spans="1:6">
+      <c r="I203" t="s">
+        <v>280</v>
+      </c>
+      <c r="J203" t="s">
+        <v>16</v>
+      </c>
+      <c r="K203" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L203" t="s">
+        <v>17</v>
+      </c>
+      <c r="M203" s="1">
+        <v>41609</v>
+      </c>
+      <c r="N203" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P203" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="204" spans="1:16">
       <c r="A204" t="s">
         <v>16</v>
       </c>
@@ -5287,8 +6348,29 @@
       <c r="F204" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="205" spans="1:6">
+      <c r="I204" t="s">
+        <v>280</v>
+      </c>
+      <c r="J204" t="s">
+        <v>16</v>
+      </c>
+      <c r="K204" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L204" t="s">
+        <v>17</v>
+      </c>
+      <c r="M204" s="1">
+        <v>41640</v>
+      </c>
+      <c r="N204" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P204" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="205" spans="1:16">
       <c r="A205" t="s">
         <v>16</v>
       </c>
@@ -5307,8 +6389,29 @@
       <c r="F205" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="206" spans="1:6">
+      <c r="I205" t="s">
+        <v>280</v>
+      </c>
+      <c r="J205" t="s">
+        <v>16</v>
+      </c>
+      <c r="K205" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L205" t="s">
+        <v>17</v>
+      </c>
+      <c r="M205" s="1">
+        <v>41671</v>
+      </c>
+      <c r="N205" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P205" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="206" spans="1:16">
       <c r="A206" t="s">
         <v>16</v>
       </c>
@@ -5327,8 +6430,29 @@
       <c r="F206" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="207" spans="1:6">
+      <c r="I206" t="s">
+        <v>280</v>
+      </c>
+      <c r="J206" t="s">
+        <v>16</v>
+      </c>
+      <c r="K206" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L206" t="s">
+        <v>17</v>
+      </c>
+      <c r="M206" s="1">
+        <v>41699</v>
+      </c>
+      <c r="N206" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P206" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="207" spans="1:16">
       <c r="A207" t="s">
         <v>16</v>
       </c>
@@ -5347,8 +6471,29 @@
       <c r="F207" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="208" spans="1:6">
+      <c r="I207" t="s">
+        <v>280</v>
+      </c>
+      <c r="J207" t="s">
+        <v>16</v>
+      </c>
+      <c r="K207" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L207" t="s">
+        <v>17</v>
+      </c>
+      <c r="M207" s="1">
+        <v>41730</v>
+      </c>
+      <c r="N207" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P207" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="208" spans="1:16">
       <c r="A208" t="s">
         <v>16</v>
       </c>
@@ -5367,8 +6512,29 @@
       <c r="F208" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="209" spans="1:6">
+      <c r="I208" t="s">
+        <v>280</v>
+      </c>
+      <c r="J208" t="s">
+        <v>16</v>
+      </c>
+      <c r="K208" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L208" t="s">
+        <v>17</v>
+      </c>
+      <c r="M208" s="1">
+        <v>41760</v>
+      </c>
+      <c r="N208" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P208" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="209" spans="1:16">
       <c r="A209" t="s">
         <v>16</v>
       </c>
@@ -5387,8 +6553,29 @@
       <c r="F209" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="210" spans="1:6">
+      <c r="I209" t="s">
+        <v>280</v>
+      </c>
+      <c r="J209" t="s">
+        <v>16</v>
+      </c>
+      <c r="K209" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L209" t="s">
+        <v>17</v>
+      </c>
+      <c r="M209" s="1">
+        <v>41791</v>
+      </c>
+      <c r="N209" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P209" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="210" spans="1:16">
       <c r="A210" t="s">
         <v>16</v>
       </c>
@@ -5407,8 +6594,29 @@
       <c r="F210" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="211" spans="1:6">
+      <c r="I210" t="s">
+        <v>280</v>
+      </c>
+      <c r="J210" t="s">
+        <v>16</v>
+      </c>
+      <c r="K210" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L210" t="s">
+        <v>17</v>
+      </c>
+      <c r="M210" s="1">
+        <v>41821</v>
+      </c>
+      <c r="N210" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P210" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="211" spans="1:16">
       <c r="A211" t="s">
         <v>16</v>
       </c>
@@ -5427,8 +6635,29 @@
       <c r="F211" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="212" spans="1:6">
+      <c r="I211" t="s">
+        <v>280</v>
+      </c>
+      <c r="J211" t="s">
+        <v>16</v>
+      </c>
+      <c r="K211" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L211" t="s">
+        <v>17</v>
+      </c>
+      <c r="M211" s="1">
+        <v>41852</v>
+      </c>
+      <c r="N211" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P211" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="212" spans="1:16">
       <c r="A212" t="s">
         <v>16</v>
       </c>
@@ -5447,8 +6676,29 @@
       <c r="F212" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="213" spans="1:6">
+      <c r="I212" t="s">
+        <v>280</v>
+      </c>
+      <c r="J212" t="s">
+        <v>16</v>
+      </c>
+      <c r="K212" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L212" t="s">
+        <v>17</v>
+      </c>
+      <c r="M212" s="1">
+        <v>41883</v>
+      </c>
+      <c r="N212" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P212" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="213" spans="1:16">
       <c r="A213" t="s">
         <v>16</v>
       </c>
@@ -5467,8 +6717,29 @@
       <c r="F213" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="214" spans="1:6">
+      <c r="I213" t="s">
+        <v>280</v>
+      </c>
+      <c r="J213" t="s">
+        <v>16</v>
+      </c>
+      <c r="K213" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L213" t="s">
+        <v>17</v>
+      </c>
+      <c r="M213" s="1">
+        <v>41913</v>
+      </c>
+      <c r="N213" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P213" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="214" spans="1:16">
       <c r="A214" t="s">
         <v>16</v>
       </c>
@@ -5487,8 +6758,29 @@
       <c r="F214" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="215" spans="1:6">
+      <c r="I214" t="s">
+        <v>280</v>
+      </c>
+      <c r="J214" t="s">
+        <v>16</v>
+      </c>
+      <c r="K214" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L214" t="s">
+        <v>17</v>
+      </c>
+      <c r="M214" s="1">
+        <v>41944</v>
+      </c>
+      <c r="N214" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P214" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="215" spans="1:16">
       <c r="A215" t="s">
         <v>16</v>
       </c>
@@ -5507,8 +6799,29 @@
       <c r="F215" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="216" spans="1:6">
+      <c r="I215" t="s">
+        <v>280</v>
+      </c>
+      <c r="J215" t="s">
+        <v>16</v>
+      </c>
+      <c r="K215" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L215" t="s">
+        <v>17</v>
+      </c>
+      <c r="M215" s="1">
+        <v>41974</v>
+      </c>
+      <c r="N215" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P215" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="216" spans="1:16">
       <c r="A216" t="s">
         <v>16</v>
       </c>
@@ -5527,8 +6840,29 @@
       <c r="F216" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="217" spans="1:6">
+      <c r="I216" t="s">
+        <v>280</v>
+      </c>
+      <c r="J216" t="s">
+        <v>16</v>
+      </c>
+      <c r="K216" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L216" t="s">
+        <v>17</v>
+      </c>
+      <c r="M216" s="1">
+        <v>42005</v>
+      </c>
+      <c r="N216" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P216" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="217" spans="1:16">
       <c r="A217" t="s">
         <v>16</v>
       </c>
@@ -5547,8 +6881,29 @@
       <c r="F217" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="218" spans="1:6">
+      <c r="I217" t="s">
+        <v>280</v>
+      </c>
+      <c r="J217" t="s">
+        <v>16</v>
+      </c>
+      <c r="K217" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L217" t="s">
+        <v>17</v>
+      </c>
+      <c r="M217" s="1">
+        <v>42036</v>
+      </c>
+      <c r="N217" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P217" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="218" spans="1:16">
       <c r="A218" t="s">
         <v>16</v>
       </c>
@@ -5567,8 +6922,29 @@
       <c r="F218" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="219" spans="1:6">
+      <c r="I218" t="s">
+        <v>280</v>
+      </c>
+      <c r="J218" t="s">
+        <v>16</v>
+      </c>
+      <c r="K218" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L218" t="s">
+        <v>17</v>
+      </c>
+      <c r="M218" s="1">
+        <v>42064</v>
+      </c>
+      <c r="N218" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P218" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="219" spans="1:16">
       <c r="A219" t="s">
         <v>16</v>
       </c>
@@ -5587,8 +6963,29 @@
       <c r="F219" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="220" spans="1:6">
+      <c r="I219" t="s">
+        <v>280</v>
+      </c>
+      <c r="J219" t="s">
+        <v>16</v>
+      </c>
+      <c r="K219" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L219" t="s">
+        <v>17</v>
+      </c>
+      <c r="M219" s="1">
+        <v>42095</v>
+      </c>
+      <c r="N219" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P219" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="220" spans="1:16">
       <c r="A220" t="s">
         <v>16</v>
       </c>
@@ -5607,8 +7004,29 @@
       <c r="F220" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="221" spans="1:6">
+      <c r="I220" t="s">
+        <v>280</v>
+      </c>
+      <c r="J220" t="s">
+        <v>16</v>
+      </c>
+      <c r="K220" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L220" t="s">
+        <v>17</v>
+      </c>
+      <c r="M220" s="1">
+        <v>42125</v>
+      </c>
+      <c r="N220" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P220" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="221" spans="1:16">
       <c r="A221" t="s">
         <v>16</v>
       </c>
@@ -5627,8 +7045,29 @@
       <c r="F221" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="222" spans="1:6">
+      <c r="I221" t="s">
+        <v>280</v>
+      </c>
+      <c r="J221" t="s">
+        <v>16</v>
+      </c>
+      <c r="K221" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L221" t="s">
+        <v>17</v>
+      </c>
+      <c r="M221" s="1">
+        <v>42156</v>
+      </c>
+      <c r="N221" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P221" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="222" spans="1:16">
       <c r="A222" t="s">
         <v>16</v>
       </c>
@@ -5647,8 +7086,29 @@
       <c r="F222" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="223" spans="1:6">
+      <c r="I222" t="s">
+        <v>280</v>
+      </c>
+      <c r="J222" t="s">
+        <v>16</v>
+      </c>
+      <c r="K222" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L222" t="s">
+        <v>17</v>
+      </c>
+      <c r="M222" s="1">
+        <v>42186</v>
+      </c>
+      <c r="N222" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P222" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="223" spans="1:16">
       <c r="A223" t="s">
         <v>16</v>
       </c>
@@ -5667,8 +7127,29 @@
       <c r="F223" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="224" spans="1:6">
+      <c r="I223" t="s">
+        <v>280</v>
+      </c>
+      <c r="J223" t="s">
+        <v>16</v>
+      </c>
+      <c r="K223" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L223" t="s">
+        <v>17</v>
+      </c>
+      <c r="M223" s="1">
+        <v>42217</v>
+      </c>
+      <c r="N223" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P223" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="224" spans="1:16">
       <c r="A224" t="s">
         <v>16</v>
       </c>
@@ -5687,8 +7168,29 @@
       <c r="F224" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="225" spans="1:6">
+      <c r="I224" t="s">
+        <v>280</v>
+      </c>
+      <c r="J224" t="s">
+        <v>16</v>
+      </c>
+      <c r="K224" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L224" t="s">
+        <v>17</v>
+      </c>
+      <c r="M224" s="1">
+        <v>42248</v>
+      </c>
+      <c r="N224" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P224" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="225" spans="1:16">
       <c r="A225" t="s">
         <v>16</v>
       </c>
@@ -5707,8 +7209,29 @@
       <c r="F225" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="226" spans="1:6">
+      <c r="I225" t="s">
+        <v>280</v>
+      </c>
+      <c r="J225" t="s">
+        <v>16</v>
+      </c>
+      <c r="K225" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L225" t="s">
+        <v>17</v>
+      </c>
+      <c r="M225" s="1">
+        <v>42278</v>
+      </c>
+      <c r="N225" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P225" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="226" spans="1:16">
       <c r="A226" t="s">
         <v>16</v>
       </c>
@@ -5727,8 +7250,29 @@
       <c r="F226" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="227" spans="1:6">
+      <c r="I226" t="s">
+        <v>280</v>
+      </c>
+      <c r="J226" t="s">
+        <v>16</v>
+      </c>
+      <c r="K226" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L226" t="s">
+        <v>17</v>
+      </c>
+      <c r="M226" s="1">
+        <v>42309</v>
+      </c>
+      <c r="N226" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P226" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="227" spans="1:16">
       <c r="A227" t="s">
         <v>16</v>
       </c>
@@ -5747,8 +7291,29 @@
       <c r="F227" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="228" spans="1:6">
+      <c r="I227" t="s">
+        <v>280</v>
+      </c>
+      <c r="J227" t="s">
+        <v>16</v>
+      </c>
+      <c r="K227" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L227" t="s">
+        <v>17</v>
+      </c>
+      <c r="M227" s="1">
+        <v>42339</v>
+      </c>
+      <c r="N227" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P227" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="228" spans="1:16">
       <c r="A228" t="s">
         <v>16</v>
       </c>
@@ -5767,8 +7332,29 @@
       <c r="F228" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="229" spans="1:6">
+      <c r="I228" t="s">
+        <v>280</v>
+      </c>
+      <c r="J228" t="s">
+        <v>16</v>
+      </c>
+      <c r="K228" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L228" t="s">
+        <v>17</v>
+      </c>
+      <c r="M228" s="1">
+        <v>42370</v>
+      </c>
+      <c r="N228" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P228" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="229" spans="1:16">
       <c r="A229" t="s">
         <v>16</v>
       </c>
@@ -5787,8 +7373,29 @@
       <c r="F229" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="230" spans="1:6">
+      <c r="I229" t="s">
+        <v>280</v>
+      </c>
+      <c r="J229" t="s">
+        <v>16</v>
+      </c>
+      <c r="K229" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L229" t="s">
+        <v>17</v>
+      </c>
+      <c r="M229" s="1">
+        <v>42401</v>
+      </c>
+      <c r="N229" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P229" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="230" spans="1:16">
       <c r="A230" t="s">
         <v>16</v>
       </c>
@@ -5807,8 +7414,29 @@
       <c r="F230" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="231" spans="1:6">
+      <c r="I230" t="s">
+        <v>280</v>
+      </c>
+      <c r="J230" t="s">
+        <v>16</v>
+      </c>
+      <c r="K230" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L230" t="s">
+        <v>17</v>
+      </c>
+      <c r="M230" s="1">
+        <v>42430</v>
+      </c>
+      <c r="N230" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P230" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="231" spans="1:16">
       <c r="A231" t="s">
         <v>16</v>
       </c>
@@ -5827,8 +7455,29 @@
       <c r="F231" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="232" spans="1:6">
+      <c r="I231" t="s">
+        <v>280</v>
+      </c>
+      <c r="J231" t="s">
+        <v>16</v>
+      </c>
+      <c r="K231" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L231" t="s">
+        <v>17</v>
+      </c>
+      <c r="M231" s="1">
+        <v>42461</v>
+      </c>
+      <c r="N231" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P231" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="232" spans="1:16">
       <c r="A232" t="s">
         <v>16</v>
       </c>
@@ -5847,8 +7496,29 @@
       <c r="F232" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="233" spans="1:6">
+      <c r="I232" t="s">
+        <v>280</v>
+      </c>
+      <c r="J232" t="s">
+        <v>16</v>
+      </c>
+      <c r="K232" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L232" t="s">
+        <v>17</v>
+      </c>
+      <c r="M232" s="1">
+        <v>42491</v>
+      </c>
+      <c r="N232" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P232" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="233" spans="1:16">
       <c r="A233" t="s">
         <v>16</v>
       </c>
@@ -5867,8 +7537,29 @@
       <c r="F233" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="234" spans="1:6">
+      <c r="I233" t="s">
+        <v>280</v>
+      </c>
+      <c r="J233" t="s">
+        <v>16</v>
+      </c>
+      <c r="K233" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L233" t="s">
+        <v>17</v>
+      </c>
+      <c r="M233" s="1">
+        <v>42522</v>
+      </c>
+      <c r="N233" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P233" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="234" spans="1:16">
       <c r="A234" t="s">
         <v>16</v>
       </c>
@@ -5887,8 +7578,29 @@
       <c r="F234" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="235" spans="1:6">
+      <c r="I234" t="s">
+        <v>280</v>
+      </c>
+      <c r="J234" t="s">
+        <v>16</v>
+      </c>
+      <c r="K234" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L234" t="s">
+        <v>17</v>
+      </c>
+      <c r="M234" s="1">
+        <v>42552</v>
+      </c>
+      <c r="N234" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P234" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="235" spans="1:16">
       <c r="A235" t="s">
         <v>16</v>
       </c>
@@ -5907,8 +7619,29 @@
       <c r="F235" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="236" spans="1:6">
+      <c r="I235" t="s">
+        <v>280</v>
+      </c>
+      <c r="J235" t="s">
+        <v>16</v>
+      </c>
+      <c r="K235" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L235" t="s">
+        <v>17</v>
+      </c>
+      <c r="M235" s="1">
+        <v>42583</v>
+      </c>
+      <c r="N235" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P235" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="236" spans="1:16">
       <c r="A236" t="s">
         <v>16</v>
       </c>
@@ -5927,8 +7660,29 @@
       <c r="F236" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="237" spans="1:6">
+      <c r="I236" t="s">
+        <v>280</v>
+      </c>
+      <c r="J236" t="s">
+        <v>16</v>
+      </c>
+      <c r="K236" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L236" t="s">
+        <v>17</v>
+      </c>
+      <c r="M236" s="1">
+        <v>42614</v>
+      </c>
+      <c r="N236" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P236" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="237" spans="1:16">
       <c r="A237" t="s">
         <v>16</v>
       </c>
@@ -5947,8 +7701,29 @@
       <c r="F237" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="238" spans="1:6">
+      <c r="I237" t="s">
+        <v>280</v>
+      </c>
+      <c r="J237" t="s">
+        <v>16</v>
+      </c>
+      <c r="K237" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L237" t="s">
+        <v>17</v>
+      </c>
+      <c r="M237" s="1">
+        <v>42644</v>
+      </c>
+      <c r="N237" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P237" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="238" spans="1:16">
       <c r="A238" t="s">
         <v>16</v>
       </c>
@@ -5967,8 +7742,29 @@
       <c r="F238" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="239" spans="1:6">
+      <c r="I238" t="s">
+        <v>280</v>
+      </c>
+      <c r="J238" t="s">
+        <v>16</v>
+      </c>
+      <c r="K238" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L238" t="s">
+        <v>17</v>
+      </c>
+      <c r="M238" s="1">
+        <v>42675</v>
+      </c>
+      <c r="N238" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P238" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="239" spans="1:16">
       <c r="A239" t="s">
         <v>16</v>
       </c>
@@ -5987,8 +7783,29 @@
       <c r="F239" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="240" spans="1:6">
+      <c r="I239" t="s">
+        <v>280</v>
+      </c>
+      <c r="J239" t="s">
+        <v>16</v>
+      </c>
+      <c r="K239" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L239" t="s">
+        <v>17</v>
+      </c>
+      <c r="M239" s="1">
+        <v>42705</v>
+      </c>
+      <c r="N239" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P239" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="240" spans="1:16">
       <c r="A240" t="s">
         <v>16</v>
       </c>
@@ -6007,8 +7824,29 @@
       <c r="F240" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="241" spans="1:6">
+      <c r="I240" t="s">
+        <v>280</v>
+      </c>
+      <c r="J240" t="s">
+        <v>16</v>
+      </c>
+      <c r="K240" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L240" t="s">
+        <v>17</v>
+      </c>
+      <c r="M240" s="1">
+        <v>42736</v>
+      </c>
+      <c r="N240" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P240" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="241" spans="1:16">
       <c r="A241" t="s">
         <v>16</v>
       </c>
@@ -6027,8 +7865,29 @@
       <c r="F241" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="242" spans="1:6">
+      <c r="I241" t="s">
+        <v>280</v>
+      </c>
+      <c r="J241" t="s">
+        <v>16</v>
+      </c>
+      <c r="K241" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L241" t="s">
+        <v>17</v>
+      </c>
+      <c r="M241" s="1">
+        <v>42767</v>
+      </c>
+      <c r="N241" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P241" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="242" spans="1:16">
       <c r="A242" t="s">
         <v>16</v>
       </c>
@@ -6047,8 +7906,29 @@
       <c r="F242" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="243" spans="1:6">
+      <c r="I242" t="s">
+        <v>280</v>
+      </c>
+      <c r="J242" t="s">
+        <v>16</v>
+      </c>
+      <c r="K242" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L242" t="s">
+        <v>17</v>
+      </c>
+      <c r="M242" s="1">
+        <v>42795</v>
+      </c>
+      <c r="N242" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P242" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="243" spans="1:16">
       <c r="A243" t="s">
         <v>16</v>
       </c>
@@ -6067,8 +7947,29 @@
       <c r="F243" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="244" spans="1:6">
+      <c r="I243" t="s">
+        <v>280</v>
+      </c>
+      <c r="J243" t="s">
+        <v>16</v>
+      </c>
+      <c r="K243" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L243" t="s">
+        <v>17</v>
+      </c>
+      <c r="M243" s="1">
+        <v>42826</v>
+      </c>
+      <c r="N243" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P243" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="244" spans="1:16">
       <c r="A244" t="s">
         <v>16</v>
       </c>
@@ -6087,8 +7988,29 @@
       <c r="F244" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="245" spans="1:6">
+      <c r="I244" t="s">
+        <v>280</v>
+      </c>
+      <c r="J244" t="s">
+        <v>16</v>
+      </c>
+      <c r="K244" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L244" t="s">
+        <v>17</v>
+      </c>
+      <c r="M244" s="1">
+        <v>42856</v>
+      </c>
+      <c r="N244" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P244" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="245" spans="1:16">
       <c r="A245" t="s">
         <v>16</v>
       </c>
@@ -6107,8 +8029,29 @@
       <c r="F245" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="246" spans="1:6">
+      <c r="I245" t="s">
+        <v>280</v>
+      </c>
+      <c r="J245" t="s">
+        <v>16</v>
+      </c>
+      <c r="K245" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L245" t="s">
+        <v>17</v>
+      </c>
+      <c r="M245" s="1">
+        <v>42887</v>
+      </c>
+      <c r="N245" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P245" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="246" spans="1:16">
       <c r="A246" t="s">
         <v>16</v>
       </c>
@@ -6127,8 +8070,29 @@
       <c r="F246" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="247" spans="1:6">
+      <c r="I246" t="s">
+        <v>280</v>
+      </c>
+      <c r="J246" t="s">
+        <v>16</v>
+      </c>
+      <c r="K246" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="L246" t="s">
+        <v>17</v>
+      </c>
+      <c r="M246" s="1">
+        <v>42917</v>
+      </c>
+      <c r="N246" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P246" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="247" spans="1:16">
       <c r="A247" t="s">
         <v>16</v>
       </c>
@@ -6147,8 +8111,29 @@
       <c r="F247" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="248" spans="1:6">
+      <c r="I247" t="s">
+        <v>280</v>
+      </c>
+      <c r="J247" t="s">
+        <v>16</v>
+      </c>
+      <c r="K247" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L247" t="s">
+        <v>17</v>
+      </c>
+      <c r="M247" s="1">
+        <v>42948</v>
+      </c>
+      <c r="N247" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P247" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="248" spans="1:16">
       <c r="A248" t="s">
         <v>16</v>
       </c>
@@ -6167,8 +8152,29 @@
       <c r="F248" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="249" spans="1:6">
+      <c r="I248" t="s">
+        <v>280</v>
+      </c>
+      <c r="J248" t="s">
+        <v>16</v>
+      </c>
+      <c r="K248" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L248" t="s">
+        <v>17</v>
+      </c>
+      <c r="M248" s="1">
+        <v>42979</v>
+      </c>
+      <c r="N248" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P248" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="249" spans="1:16">
       <c r="A249" t="s">
         <v>16</v>
       </c>
@@ -6187,8 +8193,29 @@
       <c r="F249" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="250" spans="1:6">
+      <c r="I249" t="s">
+        <v>280</v>
+      </c>
+      <c r="J249" t="s">
+        <v>16</v>
+      </c>
+      <c r="K249" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="L249" t="s">
+        <v>17</v>
+      </c>
+      <c r="M249" s="1">
+        <v>43009</v>
+      </c>
+      <c r="N249" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P249" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="250" spans="1:16">
       <c r="A250" t="s">
         <v>16</v>
       </c>
@@ -6207,8 +8234,29 @@
       <c r="F250" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="251" spans="1:6">
+      <c r="I250" t="s">
+        <v>280</v>
+      </c>
+      <c r="J250" t="s">
+        <v>16</v>
+      </c>
+      <c r="K250" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L250" t="s">
+        <v>17</v>
+      </c>
+      <c r="M250" s="1">
+        <v>43040</v>
+      </c>
+      <c r="N250" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P250" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="251" spans="1:16">
       <c r="A251" t="s">
         <v>16</v>
       </c>
@@ -6227,8 +8275,29 @@
       <c r="F251" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="252" spans="1:6">
+      <c r="I251" t="s">
+        <v>280</v>
+      </c>
+      <c r="J251" t="s">
+        <v>16</v>
+      </c>
+      <c r="K251" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L251" t="s">
+        <v>17</v>
+      </c>
+      <c r="M251" s="1">
+        <v>43070</v>
+      </c>
+      <c r="N251" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P251" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="252" spans="1:16">
       <c r="A252" t="s">
         <v>16</v>
       </c>
@@ -6247,8 +8316,29 @@
       <c r="F252" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="253" spans="1:6">
+      <c r="I252" t="s">
+        <v>280</v>
+      </c>
+      <c r="J252" t="s">
+        <v>16</v>
+      </c>
+      <c r="K252" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L252" t="s">
+        <v>17</v>
+      </c>
+      <c r="M252" s="1">
+        <v>43101</v>
+      </c>
+      <c r="N252" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P252" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="253" spans="1:16">
       <c r="A253" t="s">
         <v>16</v>
       </c>
@@ -6267,8 +8357,29 @@
       <c r="F253" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="254" spans="1:6">
+      <c r="I253" t="s">
+        <v>280</v>
+      </c>
+      <c r="J253" t="s">
+        <v>16</v>
+      </c>
+      <c r="K253" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="L253" t="s">
+        <v>17</v>
+      </c>
+      <c r="M253" s="1">
+        <v>43132</v>
+      </c>
+      <c r="N253" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P253" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="254" spans="1:16">
       <c r="A254" t="s">
         <v>16</v>
       </c>
@@ -6287,8 +8398,29 @@
       <c r="F254" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="255" spans="1:6">
+      <c r="I254" t="s">
+        <v>280</v>
+      </c>
+      <c r="J254" t="s">
+        <v>16</v>
+      </c>
+      <c r="K254" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="L254" t="s">
+        <v>17</v>
+      </c>
+      <c r="M254" s="1">
+        <v>43160</v>
+      </c>
+      <c r="N254" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P254" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="255" spans="1:16">
       <c r="A255" t="s">
         <v>16</v>
       </c>
@@ -6307,8 +8439,29 @@
       <c r="F255" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="256" spans="1:6">
+      <c r="I255" t="s">
+        <v>280</v>
+      </c>
+      <c r="J255" t="s">
+        <v>16</v>
+      </c>
+      <c r="K255" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L255" t="s">
+        <v>17</v>
+      </c>
+      <c r="M255" s="1">
+        <v>43191</v>
+      </c>
+      <c r="N255" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P255" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="256" spans="1:16">
       <c r="A256" t="s">
         <v>16</v>
       </c>
@@ -6327,8 +8480,29 @@
       <c r="F256" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="257" spans="1:6">
+      <c r="I256" t="s">
+        <v>280</v>
+      </c>
+      <c r="J256" t="s">
+        <v>16</v>
+      </c>
+      <c r="K256" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L256" t="s">
+        <v>17</v>
+      </c>
+      <c r="M256" s="1">
+        <v>43221</v>
+      </c>
+      <c r="N256" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P256" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="257" spans="1:16">
       <c r="A257" t="s">
         <v>16</v>
       </c>
@@ -6347,8 +8521,29 @@
       <c r="F257" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="258" spans="1:6">
+      <c r="I257" t="s">
+        <v>280</v>
+      </c>
+      <c r="J257" t="s">
+        <v>16</v>
+      </c>
+      <c r="K257" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L257" t="s">
+        <v>17</v>
+      </c>
+      <c r="M257" s="1">
+        <v>43252</v>
+      </c>
+      <c r="N257" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P257" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="258" spans="1:16">
       <c r="A258" t="s">
         <v>16</v>
       </c>
@@ -6367,8 +8562,29 @@
       <c r="F258" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="259" spans="1:6">
+      <c r="I258" t="s">
+        <v>280</v>
+      </c>
+      <c r="J258" t="s">
+        <v>16</v>
+      </c>
+      <c r="K258" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L258" t="s">
+        <v>17</v>
+      </c>
+      <c r="M258" s="1">
+        <v>43282</v>
+      </c>
+      <c r="N258" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P258" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16">
       <c r="A259" t="s">
         <v>16</v>
       </c>
@@ -6387,8 +8603,29 @@
       <c r="F259" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="260" spans="1:6">
+      <c r="I259" t="s">
+        <v>280</v>
+      </c>
+      <c r="J259" t="s">
+        <v>16</v>
+      </c>
+      <c r="K259" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L259" t="s">
+        <v>17</v>
+      </c>
+      <c r="M259" s="1">
+        <v>43313</v>
+      </c>
+      <c r="N259" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P259" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="260" spans="1:16">
       <c r="A260" t="s">
         <v>16</v>
       </c>
@@ -6407,8 +8644,29 @@
       <c r="F260" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="261" spans="1:6">
+      <c r="I260" t="s">
+        <v>280</v>
+      </c>
+      <c r="J260" t="s">
+        <v>16</v>
+      </c>
+      <c r="K260" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="L260" t="s">
+        <v>17</v>
+      </c>
+      <c r="M260" s="1">
+        <v>43344</v>
+      </c>
+      <c r="N260" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P260" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16">
       <c r="A261" t="s">
         <v>16</v>
       </c>
@@ -6427,8 +8685,29 @@
       <c r="F261" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="262" spans="1:6">
+      <c r="I261" t="s">
+        <v>280</v>
+      </c>
+      <c r="J261" t="s">
+        <v>16</v>
+      </c>
+      <c r="K261" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L261" t="s">
+        <v>17</v>
+      </c>
+      <c r="M261" s="1">
+        <v>43374</v>
+      </c>
+      <c r="N261" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P261" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16">
       <c r="A262" t="s">
         <v>16</v>
       </c>
@@ -6447,8 +8726,29 @@
       <c r="F262" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="263" spans="1:6">
+      <c r="I262" t="s">
+        <v>280</v>
+      </c>
+      <c r="J262" t="s">
+        <v>16</v>
+      </c>
+      <c r="K262" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L262" t="s">
+        <v>17</v>
+      </c>
+      <c r="M262" s="1">
+        <v>43405</v>
+      </c>
+      <c r="N262" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P262" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16">
       <c r="A263" t="s">
         <v>16</v>
       </c>
@@ -6467,8 +8767,29 @@
       <c r="F263" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="264" spans="1:6">
+      <c r="I263" t="s">
+        <v>280</v>
+      </c>
+      <c r="J263" t="s">
+        <v>16</v>
+      </c>
+      <c r="K263" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="L263" t="s">
+        <v>17</v>
+      </c>
+      <c r="M263" s="1">
+        <v>43435</v>
+      </c>
+      <c r="N263" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P263" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16">
       <c r="A264" t="s">
         <v>16</v>
       </c>
@@ -6486,6 +8807,27 @@
       </c>
       <c r="F264" t="s">
         <v>30</v>
+      </c>
+      <c r="I264" t="s">
+        <v>280</v>
+      </c>
+      <c r="J264" t="s">
+        <v>16</v>
+      </c>
+      <c r="K264" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L264" t="s">
+        <v>17</v>
+      </c>
+      <c r="M264" s="1">
+        <v>43466</v>
+      </c>
+      <c r="N264" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="P264" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="282" spans="2:5">

</xml_diff>